<commit_message>
add 2021 Feb question
</commit_message>
<xml_diff>
--- a/usaco problems spreadsheet.xlsx
+++ b/usaco problems spreadsheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shiva\Documents\GitHub\USACO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/weiminding/Projects/USACO/USACO-1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C91EE5F4-528E-459C-904C-00FFE884C44D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{103A1392-92A9-0040-919F-6CD052F95274}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12360" xr2:uid="{3E9A51D4-ACA4-4110-979E-41C73A6D5C73}"/>
+    <workbookView xWindow="2220" yWindow="2780" windowWidth="28200" windowHeight="18100" xr2:uid="{3E9A51D4-ACA4-4110-979E-41C73A6D5C73}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="385">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="389">
   <si>
     <t>2012 November</t>
   </si>
@@ -1180,6 +1180,18 @@
   </si>
   <si>
     <t>NOT SOLVED AT ALL</t>
+  </si>
+  <si>
+    <t>Comfortable Cows</t>
+  </si>
+  <si>
+    <t>Year of the Cow</t>
+  </si>
+  <si>
+    <t>Just Green Enough</t>
+  </si>
+  <si>
+    <t>Clockwise Fence</t>
   </si>
 </sst>
 </file>
@@ -1593,17 +1605,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E76098A-30F6-4519-8814-8A13749239BB}">
   <dimension ref="A1:N47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+    <sheetView tabSelected="1" zoomScale="94" zoomScaleNormal="94" workbookViewId="0">
+      <selection activeCell="H43" sqref="H43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.5546875" customWidth="1"/>
-    <col min="2" max="14" width="20.77734375" customWidth="1"/>
+    <col min="1" max="1" width="22.5" customWidth="1"/>
+    <col min="2" max="14" width="20.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1644,7 +1656,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1679,7 +1691,7 @@
       <c r="M2" s="6"/>
       <c r="N2" s="6"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>21</v>
       </c>
@@ -1714,7 +1726,7 @@
       <c r="M3" s="6"/>
       <c r="N3" s="6"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>30</v>
       </c>
@@ -1749,7 +1761,7 @@
       <c r="M4" s="6"/>
       <c r="N4" s="6"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>31</v>
       </c>
@@ -1784,7 +1796,7 @@
       <c r="M5" s="6"/>
       <c r="N5" s="6"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>32</v>
       </c>
@@ -1819,7 +1831,7 @@
       <c r="M6" s="6"/>
       <c r="N6" s="6"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>33</v>
       </c>
@@ -1857,7 +1869,7 @@
       <c r="M7" s="6"/>
       <c r="N7" s="6"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>68</v>
       </c>
@@ -1892,7 +1904,7 @@
       <c r="M8" s="6"/>
       <c r="N8" s="6"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>69</v>
       </c>
@@ -1927,7 +1939,7 @@
       <c r="M9" s="6"/>
       <c r="N9" s="6"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>70</v>
       </c>
@@ -1962,7 +1974,7 @@
       <c r="M10" s="6"/>
       <c r="N10" s="6"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>71</v>
       </c>
@@ -1997,7 +2009,7 @@
       <c r="M11" s="6"/>
       <c r="N11" s="6"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>102</v>
       </c>
@@ -2032,7 +2044,7 @@
       <c r="M12" s="6"/>
       <c r="N12" s="6"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>103</v>
       </c>
@@ -2067,7 +2079,7 @@
       <c r="M13" s="6"/>
       <c r="N13" s="6"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>118</v>
       </c>
@@ -2105,7 +2117,7 @@
       <c r="M14" s="6"/>
       <c r="N14" s="6"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>119</v>
       </c>
@@ -2143,7 +2155,7 @@
       <c r="M15" s="6"/>
       <c r="N15" s="6"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>120</v>
       </c>
@@ -2178,7 +2190,7 @@
       <c r="M16" s="6"/>
       <c r="N16" s="6"/>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>121</v>
       </c>
@@ -2216,7 +2228,7 @@
       <c r="M17" s="6"/>
       <c r="N17" s="6"/>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>154</v>
       </c>
@@ -2257,7 +2269,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>155</v>
       </c>
@@ -2298,7 +2310,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>156</v>
       </c>
@@ -2339,7 +2351,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>157</v>
       </c>
@@ -2380,7 +2392,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>189</v>
       </c>
@@ -2421,7 +2433,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>190</v>
       </c>
@@ -2462,7 +2474,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>191</v>
       </c>
@@ -2503,7 +2515,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>192</v>
       </c>
@@ -2541,7 +2553,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>223</v>
       </c>
@@ -2582,7 +2594,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>224</v>
       </c>
@@ -2623,7 +2635,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>225</v>
       </c>
@@ -2664,7 +2676,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>226</v>
       </c>
@@ -2705,7 +2717,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>263</v>
       </c>
@@ -2746,7 +2758,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>264</v>
       </c>
@@ -2787,7 +2799,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>265</v>
       </c>
@@ -2828,7 +2840,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>266</v>
       </c>
@@ -2869,7 +2881,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>311</v>
       </c>
@@ -2910,7 +2922,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>312</v>
       </c>
@@ -2951,7 +2963,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>313</v>
       </c>
@@ -2992,7 +3004,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>314</v>
       </c>
@@ -3033,7 +3045,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>358</v>
       </c>
@@ -3074,7 +3086,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>359</v>
       </c>
@@ -3115,27 +3127,45 @@
         <v>381</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
         <v>360</v>
       </c>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B40" t="s">
+        <v>386</v>
+      </c>
+      <c r="C40" t="s">
+        <v>385</v>
+      </c>
+      <c r="D40" t="s">
+        <v>388</v>
+      </c>
+      <c r="F40" t="s">
+        <v>385</v>
+      </c>
+      <c r="G40" t="s">
+        <v>386</v>
+      </c>
+      <c r="H40" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
         <v>382</v>
       </c>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A46" s="4" t="s">
         <v>383</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A47" s="5" t="s">
         <v>384</v>
       </c>

</xml_diff>